<commit_message>
accurate orbiter model included in aocs sizing
</commit_message>
<xml_diff>
--- a/geometry.xlsx
+++ b/geometry.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11580" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11580" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Calculations Rough Input" sheetId="1" r:id="rId1"/>
     <sheet name="TTC" sheetId="3" r:id="rId2"/>
-    <sheet name="Thrusters" sheetId="2" r:id="rId3"/>
+    <sheet name="EPS" sheetId="5" r:id="rId3"/>
+    <sheet name="Fuel" sheetId="4" r:id="rId4"/>
+    <sheet name="Thrusters" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="61">
   <si>
     <t>Solar Array</t>
   </si>
@@ -106,15 +108,6 @@
     <t>z-</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
     <t>face1</t>
   </si>
   <si>
@@ -128,6 +121,96 @@
   </si>
   <si>
     <t>offset2</t>
+  </si>
+  <si>
+    <t>att1</t>
+  </si>
+  <si>
+    <t>att2</t>
+  </si>
+  <si>
+    <t>att3</t>
+  </si>
+  <si>
+    <t>att4</t>
+  </si>
+  <si>
+    <t>att5</t>
+  </si>
+  <si>
+    <t>att6</t>
+  </si>
+  <si>
+    <t>att7</t>
+  </si>
+  <si>
+    <t>att8</t>
+  </si>
+  <si>
+    <t>att9</t>
+  </si>
+  <si>
+    <t>att10</t>
+  </si>
+  <si>
+    <t>att11</t>
+  </si>
+  <si>
+    <t>att12</t>
+  </si>
+  <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t>see sub_output</t>
+  </si>
+  <si>
+    <t>fuel1</t>
+  </si>
+  <si>
+    <t>fuel2</t>
+  </si>
+  <si>
+    <t>fuel3</t>
+  </si>
+  <si>
+    <t>fuel4</t>
+  </si>
+  <si>
+    <t>sa1</t>
+  </si>
+  <si>
+    <t>sa2</t>
+  </si>
+  <si>
+    <t>total mass</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>total area</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>st area</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>NOTE:  positive offset = outside body;   negative offset = inside body</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>TTC-nadir</t>
+  </si>
+  <si>
+    <t>TTC-earth</t>
   </si>
 </sst>
 </file>
@@ -171,9 +254,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M18"/>
+  <dimension ref="B1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:D30"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,6 +559,12 @@
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
       <c r="F2" t="s">
         <v>2</v>
       </c>
@@ -483,6 +573,12 @@
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
@@ -491,6 +587,12 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
       <c r="E4">
         <v>1</v>
       </c>
@@ -515,6 +617,13 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5">
+        <f>C2/2</f>
+        <v>6</v>
+      </c>
       <c r="E5">
         <v>1</v>
       </c>
@@ -539,6 +648,13 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6">
+        <f>2*SQRT(C5/2)</f>
+        <v>3.4641016151377544</v>
+      </c>
       <c r="E6">
         <v>1</v>
       </c>
@@ -563,6 +679,13 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7">
+        <f>SQRT(C5/2)</f>
+        <v>1.7320508075688772</v>
+      </c>
       <c r="E7">
         <v>3</v>
       </c>
@@ -576,13 +699,6 @@
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="1">
-        <f>SUM(L4:L6)</f>
-        <v>11.6</v>
-      </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E8">
@@ -598,9 +714,6 @@
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="K8" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="G9" s="1" t="s">
@@ -610,14 +723,12 @@
         <f>SUM(H4:H8)</f>
         <v>45.3</v>
       </c>
-      <c r="K9" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9">
-        <v>0.5</v>
-      </c>
-      <c r="M9" t="s">
-        <v>18</v>
+      <c r="K9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="1">
+        <f>SUM(L4:L6)</f>
+        <v>11.6</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -627,21 +738,22 @@
       <c r="H10" t="s">
         <v>16</v>
       </c>
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" t="s">
-        <v>28</v>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11">
+        <v>0.5</v>
+      </c>
+      <c r="M11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -652,34 +764,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
@@ -688,22 +812,46 @@
         <v>24</v>
       </c>
       <c r="D2">
-        <v>-0.75</v>
+        <v>0.75</v>
       </c>
       <c r="E2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>'Calculations Rough Input'!H9</f>
+        <v>45.3</v>
+      </c>
+      <c r="G2">
+        <f>1.5^2</f>
+        <v>2.25</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="D3">
-        <v>-0.5</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>'Calculations Rough Input'!L9</f>
+        <v>11.6</v>
+      </c>
+      <c r="G3">
+        <f>0.42*0.5</f>
+        <v>0.21</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -712,37 +860,262 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>29</v>
       </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <f>'Calculations Rough Input'!C6/2 + 0.2</f>
+        <v>1.9320508075688771</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>'Calculations Rough Input'!C$3/2</f>
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <f>'Calculations Rough Input'!C6/2 + 0.2</f>
+        <v>1.9320508075688771</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>'Calculations Rough Input'!C$3/2</f>
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>-0.35</v>
+      </c>
+      <c r="E2">
+        <v>-0.35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>-0.35</v>
+      </c>
+      <c r="E3">
+        <v>-0.35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>-0.35</v>
+      </c>
+      <c r="E4">
+        <v>-0.35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>-0.35</v>
+      </c>
+      <c r="E5">
+        <v>-0.35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
       </c>
       <c r="F1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -750,13 +1123,23 @@
       <c r="C2" t="s">
         <v>23</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
       <c r="F2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -764,13 +1147,23 @@
       <c r="C3" t="s">
         <v>22</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
       <c r="F3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -778,13 +1171,23 @@
       <c r="C4" t="s">
         <v>23</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
       <c r="F4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -792,13 +1195,22 @@
       <c r="C5" t="s">
         <v>22</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
       <c r="F5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -806,13 +1218,22 @@
       <c r="C6" t="s">
         <v>24</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
       <c r="F6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -820,13 +1241,22 @@
       <c r="C7" t="s">
         <v>25</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
       <c r="F7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
@@ -834,13 +1264,22 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
       <c r="F8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
+      <c r="G8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
@@ -848,13 +1287,22 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
       <c r="F9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
+      <c r="G9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>
@@ -862,13 +1310,22 @@
       <c r="C10" t="s">
         <v>20</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
       <c r="F10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
@@ -876,13 +1333,22 @@
       <c r="C11" t="s">
         <v>21</v>
       </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
       <c r="F11">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -890,13 +1356,22 @@
       <c r="C12" t="s">
         <v>20</v>
       </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
       <c r="F12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
@@ -904,8 +1379,17 @@
       <c r="C13" t="s">
         <v>21</v>
       </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
       <c r="F13">
         <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>